<commit_message>
Adds missing parts to BOM
</commit_message>
<xml_diff>
--- a/Spankulator.xlsx
+++ b/Spankulator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shannon\Dropbox\moog\spankulator\Spankulator-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910627F4-7EEB-4144-95BA-0DD91584A1CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957DA3D6-3C32-4DDB-87F4-CCDC940075CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
   <si>
     <t>Reference</t>
   </si>
@@ -418,6 +418,24 @@
   </si>
   <si>
     <t>1722-1241-ND</t>
+  </si>
+  <si>
+    <t>SK6</t>
+  </si>
+  <si>
+    <t>Fram header pins</t>
+  </si>
+  <si>
+    <t>732-5321-ND</t>
+  </si>
+  <si>
+    <t>N1-5</t>
+  </si>
+  <si>
+    <t>HEX NUT 0.197" NYLON M2.5</t>
+  </si>
+  <si>
+    <t>36-4687-ND</t>
   </si>
 </sst>
 </file>
@@ -735,16 +753,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
     <col min="4" max="4" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1364,7 +1382,36 @@
         <v>130</v>
       </c>
     </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Eurorack mounting screws
</commit_message>
<xml_diff>
--- a/Spankulator.xlsx
+++ b/Spankulator.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shannon\Dropbox\moog\spankulator\Spankulator-Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EEEEE55E-4301-4EF7-B0B0-0B7754D94266}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625CFF4E-1413-4468-AEA4-8ED87622F39D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
   <si>
     <t>Reference</t>
   </si>
@@ -482,12 +482,21 @@
   </si>
   <si>
     <t>H3CCS-1618G-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC6 SC7 SC8 SC9 </t>
+  </si>
+  <si>
+    <t>Mounting Screw</t>
+  </si>
+  <si>
+    <t>335-1156-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1332,11 +1341,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,161 +1929,175 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="D42" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D43" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="D47" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B49">
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>147</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>4</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>148</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>149</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>